<commit_message>
feat: implemented KMeans and DBScan.
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -3,19 +3,31 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="11880" windowHeight="10460"/>
+    <workbookView windowWidth="30240" windowHeight="12520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>内在指标</t>
   </si>
@@ -26,6 +38,9 @@
     <t>算法</t>
   </si>
   <si>
+    <t>split</t>
+  </si>
+  <si>
     <t>compactness</t>
   </si>
   <si>
@@ -81,12 +96,51 @@
   </si>
   <si>
     <t>{'standard_scaler': False, 'pca__n_components': 0.8, 'dbscan_eps': 2.0, 'dbscan_neighbors': 3}</t>
+  </si>
+  <si>
+    <t>划分</t>
+  </si>
+  <si>
+    <t>KMeans</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>2.4577 ± 0.4965</t>
+  </si>
+  <si>
+    <t>{'variance_threshold': 0.0018517164514591199, 'n_components': 0.7373910090293939, 'init': 'k-means++', 'algorithm': 'elkan'}</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>KMeans-手动实现</t>
+  </si>
+  <si>
+    <t>1.4348 ± 0.0359</t>
+  </si>
+  <si>
+    <t>{'variance_threshold': 0.1268705938561727, 'n_components': 0.8515831194601285, 'init': 'k-means++'}</t>
+  </si>
+  <si>
+    <t>网格划分</t>
+  </si>
+  <si>
+    <t>DBScan</t>
+  </si>
+  <si>
+    <t>2.015 ± 0.0941</t>
+  </si>
+  <si>
+    <t>{'variance_threshold': 0.1, 'n_components': 0.8, 'eps': 5, 'min_samples': 5}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -94,18 +148,18 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -116,68 +170,25 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -185,7 +196,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -193,7 +204,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -201,7 +212,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -209,15 +220,30 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -225,7 +251,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -233,14 +259,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -248,21 +274,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -276,49 +323,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -330,121 +461,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,21 +514,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -514,6 +546,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,148 +617,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -742,69 +789,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1100,38 +1147,40 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="14.6363636363636" style="2" customWidth="1"/>
-    <col min="3" max="8" width="13.5454545454545" style="3" customWidth="1"/>
-    <col min="9" max="9" width="111" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="2" max="2" width="18.3515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" style="2" customWidth="1"/>
+    <col min="4" max="9" width="13.546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="111" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8">
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="3:9">
+      <c r="C1" s="1"/>
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5"/>
       <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
-    <row r="2" ht="28" spans="2:9">
+    <row r="2" ht="34" spans="2:10">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -1149,98 +1198,244 @@
       <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="J2" s="10" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="8">
         <v>30313.005</v>
       </c>
-      <c r="D3" s="8">
+      <c r="E3" s="8">
         <v>2.706</v>
       </c>
-      <c r="E3" s="8">
+      <c r="F3" s="8">
         <v>0.099</v>
       </c>
-      <c r="F3" s="8">
+      <c r="G3" s="8">
         <v>0.202</v>
       </c>
-      <c r="G3" s="8">
+      <c r="H3" s="8">
         <v>0.513</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="11" t="s">
         <v>13</v>
       </c>
+      <c r="J3" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:10">
       <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="8">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="8">
         <v>19350.019</v>
       </c>
-      <c r="D4" s="8">
+      <c r="E4" s="8">
         <v>3.53</v>
       </c>
-      <c r="E4" s="8">
+      <c r="F4" s="8">
         <v>0.275</v>
       </c>
-      <c r="F4" s="8">
+      <c r="G4" s="8">
         <v>0.266</v>
       </c>
-      <c r="G4" s="8">
+      <c r="H4" s="8">
         <v>0.525</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>16</v>
       </c>
+      <c r="J4" s="13" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="8">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="8">
         <v>24387.328</v>
       </c>
-      <c r="D5" s="8">
+      <c r="E5" s="8">
         <v>3.869</v>
       </c>
-      <c r="E5" s="8">
+      <c r="F5" s="8">
         <v>0.504</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="8">
+      <c r="G5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="8">
         <v>0.33</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="12" t="s">
         <v>21</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3">
+        <v>8.9134</v>
+      </c>
+      <c r="E6" s="3">
+        <v>9.0653</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.2449</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.5482</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.4287</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3">
+        <v>8.403</v>
+      </c>
+      <c r="E7" s="3">
+        <v>9.0653</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.265</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.565</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.4472</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" ht="34" spans="2:10">
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3">
+        <v>11.871</v>
+      </c>
+      <c r="E8" s="3">
+        <v>9.1501</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.1847</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.5457</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.4095</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3">
+        <v>11.2917</v>
+      </c>
+      <c r="E9" s="3">
+        <v>9.1501</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.1853</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.5758</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.4216</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" ht="17" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="3">
+        <v>-0.353</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.348</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.085</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:G1"/>
+  <mergeCells count="9">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
updating EDA Density Hierarchical
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="11880" windowHeight="10460"/>
+    <workbookView windowWidth="12100" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,16 +53,16 @@
     <t>Agglo</t>
   </si>
   <si>
-    <t>1.25 ± 0.57</t>
-  </si>
-  <si>
-    <t>{'standard_scaler': False, 'pca__n_components': 0.99, 'agglomerative__affinity': 'euclidean', 'agglomerative__linkage': 'ward'}</t>
+    <t>2.04 ± 0.06</t>
+  </si>
+  <si>
+    <t>{'standard_scaler': False, 'pca__n_components': 0.8, 'agglomerative__affinity': 'euclidean', 'agglomerative__linkage': 'ward'}</t>
   </si>
   <si>
     <t>BIRCH</t>
   </si>
   <si>
-    <t>1.93 ± 0.68</t>
+    <t>0.85 ± 0.03</t>
   </si>
   <si>
     <t>{'standard_scaler': False, 'pca__n_components': 0.8, 'birch__threshold': 0.4, 'birch__branching_factor': 30}</t>
@@ -77,7 +77,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>11.19 ± 13.41</t>
+    <t>2.82 ± 0.08</t>
   </si>
   <si>
     <t>{'standard_scaler': False, 'pca__n_components': 0.8, 'dbscan_eps': 2.0, 'dbscan_neighbors': 3}</t>
@@ -94,7 +94,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,13 +114,6 @@
       <color rgb="FF3B3B3B"/>
       <name val="Consolas"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -570,48 +563,51 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -621,97 +617,94 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -741,9 +734,6 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -751,6 +741,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1102,8 +1093,8 @@
   <sheetPr/>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4"/>
@@ -1149,7 +1140,7 @@
       <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1161,24 +1152,24 @@
         <v>11</v>
       </c>
       <c r="C3" s="8">
-        <v>30313.005</v>
+        <v>81291.723</v>
       </c>
       <c r="D3" s="8">
-        <v>2.706</v>
+        <v>9.574</v>
       </c>
       <c r="E3" s="8">
-        <v>0.099</v>
+        <v>0.21</v>
       </c>
       <c r="F3" s="8">
-        <v>0.202</v>
+        <v>0.188</v>
       </c>
       <c r="G3" s="8">
-        <v>0.513</v>
+        <v>0.514</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1187,21 +1178,21 @@
         <v>14</v>
       </c>
       <c r="C4" s="8">
-        <v>19350.019</v>
+        <v>19257.202</v>
       </c>
       <c r="D4" s="8">
-        <v>3.53</v>
+        <v>9.005</v>
       </c>
       <c r="E4" s="8">
-        <v>0.275</v>
+        <v>0.279</v>
       </c>
       <c r="F4" s="8">
-        <v>0.266</v>
+        <v>0.27</v>
       </c>
       <c r="G4" s="8">
-        <v>0.525</v>
-      </c>
-      <c r="H4" s="10" t="s">
+        <v>0.522</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="13" t="s">
@@ -1216,24 +1207,24 @@
         <v>18</v>
       </c>
       <c r="C5" s="8">
-        <v>24387.328</v>
+        <v>129112.436</v>
       </c>
       <c r="D5" s="8">
-        <v>3.869</v>
+        <v>11.153</v>
       </c>
       <c r="E5" s="8">
-        <v>0.504</v>
-      </c>
-      <c r="F5" s="11" t="s">
+        <v>0.497</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="8">
         <v>0.33</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="12" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: implement STING method.
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -4,12 +4,25 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11910" windowHeight="10460"/>
+    <workbookView windowWidth="30240" windowHeight="12620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -115,22 +128,22 @@
     <t>{'variance_threshold': 0.1268705938561727, 'n_components': 0.8515831194601285, 'init': 'k-means++'}</t>
   </si>
   <si>
-    <t>网格划分</t>
-  </si>
-  <si>
-    <t>DBScan</t>
-  </si>
-  <si>
-    <t>2.015 ± 0.0941</t>
-  </si>
-  <si>
-    <t>{'variance_threshold': 0.1, 'n_components': 0.8, 'eps': 5, 'min_samples': 5}</t>
+    <t>网格</t>
+  </si>
+  <si>
+    <t>STING</t>
+  </si>
+  <si>
+    <t>1.795 ± 0.1532</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'variance_threshold': 0.1993592105354841, 'n_components': 0.653901865345353, 'grid_size': 6, 'density_threshold': 0.019663367994738536}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -142,14 +155,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -160,61 +173,25 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -222,7 +199,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -230,7 +207,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -238,7 +215,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -246,15 +223,30 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -262,7 +254,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -270,14 +262,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -285,21 +277,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -313,49 +326,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,121 +464,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,21 +517,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -551,6 +549,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -607,152 +620,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -782,61 +795,60 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1132,18 +1144,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="18.3545454545455" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.6363636363636" style="2" customWidth="1"/>
-    <col min="4" max="9" width="13.5454545454545" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.3515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" style="2" customWidth="1"/>
+    <col min="4" max="9" width="13.546875" style="3" customWidth="1"/>
     <col min="10" max="10" width="111" style="4" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
@@ -1161,7 +1173,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" ht="28" spans="2:10">
+    <row r="2" ht="34" spans="2:10">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1218,7 +1230,7 @@
       <c r="I3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1247,7 +1259,7 @@
       <c r="I4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1279,7 +1291,7 @@
       <c r="I5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="10" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1311,7 +1323,7 @@
       <c r="I6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1336,7 +1348,7 @@
         <v>0.4472</v>
       </c>
       <c r="I7" s="8"/>
-      <c r="J7" s="11"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="1" t="s">
@@ -1363,7 +1375,7 @@
       <c r="I8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1388,7 +1400,7 @@
         <v>0.4216</v>
       </c>
       <c r="I9" s="8"/>
-      <c r="J9" s="11"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
@@ -1398,28 +1410,29 @@
         <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="D10" s="8">
+        <v>12.413</v>
+      </c>
+      <c r="E10" s="8">
+        <v>9.795</v>
+      </c>
       <c r="F10" s="8">
-        <v>-0.353</v>
+        <v>0.2</v>
       </c>
       <c r="G10" s="8">
-        <v>0.348</v>
+        <v>0.27</v>
       </c>
       <c r="H10" s="8">
-        <v>0.085</v>
+        <v>0.077</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="10:10">
-      <c r="J11" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>